<commit_message>
Atualização Docto Mapeamento Conferência LN
</commit_message>
<xml_diff>
--- a/Documentação/Planilhas/Conferencia_CMV.xlsx
+++ b/Documentação/Planilhas/Conferencia_CMV.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
   </bookViews>
   <sheets>
     <sheet name="stg_cmv_estoque" sheetId="109" r:id="rId1"/>
@@ -407,14 +407,14 @@
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -728,7 +728,7 @@
   </sheetPr>
   <dimension ref="A1:AR28"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
   <cols>
@@ -788,10 +788,10 @@
       <c r="AR1" s="1"/>
     </row>
     <row r="2" spans="1:44" ht="21">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="10"/>
+      <c r="B2" s="11"/>
       <c r="C2" s="5" t="s">
         <v>46</v>
       </c>
@@ -807,10 +807,10 @@
       <c r="AR2" s="1"/>
     </row>
     <row r="3" spans="1:44" ht="21">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="11"/>
+      <c r="B3" s="12"/>
       <c r="C3" s="5" t="s">
         <v>85</v>
       </c>
@@ -1070,30 +1070,30 @@
       </c>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="12" t="s">
+      <c r="A18" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="B18" s="12"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="12"/>
-      <c r="B19" s="12"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
+      <c r="A19" s="10"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="12"/>
-      <c r="B20" s="12"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
+      <c r="A20" s="10"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="9" t="s">
@@ -1255,10 +1255,10 @@
       <c r="AR1" s="1"/>
     </row>
     <row r="2" spans="1:44" ht="21">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="10"/>
+      <c r="B2" s="11"/>
       <c r="C2" s="5" t="s">
         <v>4</v>
       </c>
@@ -1274,10 +1274,10 @@
       <c r="AR2" s="1"/>
     </row>
     <row r="3" spans="1:44" ht="21">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="11"/>
+      <c r="B3" s="12"/>
       <c r="C3" s="5" t="s">
         <v>29</v>
       </c>
@@ -1474,7 +1474,7 @@
   </sheetPr>
   <dimension ref="A1:AR28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
   <cols>
@@ -1534,10 +1534,10 @@
       <c r="AR1" s="1"/>
     </row>
     <row r="2" spans="1:44" ht="21">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="10"/>
+      <c r="B2" s="11"/>
       <c r="C2" s="5" t="s">
         <v>30</v>
       </c>
@@ -1553,10 +1553,10 @@
       <c r="AR2" s="1"/>
     </row>
     <row r="3" spans="1:44" ht="21">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="11"/>
+      <c r="B3" s="12"/>
       <c r="C3" s="5" t="s">
         <v>45</v>
       </c>

</xml_diff>